<commit_message>
Add remaining SOCP constraints
</commit_message>
<xml_diff>
--- a/data/example/Power_Storage.xlsx
+++ b/data/example/Power_Storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52E513-E067-4DB6-AAC2-2EA07928EEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0C254C-21C5-4D4E-B6E0-F4ED1841A017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34275" yWindow="8430" windowWidth="28800" windowHeight="15030" tabRatio="543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Storage" sheetId="106" r:id="rId1"/>
@@ -635,12 +635,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="8" builtinId="8"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -1905,55 +1905,55 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O55" sqref="O55"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="3" style="5" customWidth="1"/>
     <col min="2" max="2" width="20" style="5" customWidth="1"/>
-    <col min="3" max="4" width="13.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="5" customWidth="1"/>
-    <col min="6" max="7" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.1328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.1328125" style="5" customWidth="1"/>
+    <col min="6" max="7" width="11.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.59765625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="14.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="12" style="5" customWidth="1"/>
-    <col min="31" max="31" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="34.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="11.42578125" style="5"/>
+    <col min="39" max="16384" width="11.3984375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:37" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2047,7 +2047,7 @@
       <c r="AJ3" s="10"/>
       <c r="AK3" s="10"/>
     </row>
-    <row r="4" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E4" s="11"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -2082,7 +2082,7 @@
       <c r="AJ4" s="10"/>
       <c r="AK4" s="10"/>
     </row>
-    <row r="5" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E5" s="14"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -2117,7 +2117,7 @@
       <c r="AJ5" s="10"/>
       <c r="AK5" s="10"/>
     </row>
-    <row r="6" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:37" s="6" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E6" s="15" t="s">
         <v>20</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:37" x14ac:dyDescent="0.5">
       <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="AJ7" s="24"/>
       <c r="AK7" s="24"/>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.5">
       <c r="B8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2292,8 +2292,12 @@
       <c r="J8" s="28">
         <v>0.95</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
+      <c r="K8" s="30">
+        <v>0</v>
+      </c>
+      <c r="L8" s="30">
+        <v>0</v>
+      </c>
       <c r="M8" s="30"/>
       <c r="N8" s="29"/>
       <c r="O8" s="29"/>
@@ -2347,7 +2351,7 @@
       <c r="AJ8" s="24"/>
       <c r="AK8" s="24"/>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.5">
       <c r="B9" s="18" t="s">
         <v>35</v>
       </c>
@@ -2373,8 +2377,12 @@
       <c r="J9" s="28">
         <v>0.95</v>
       </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
+      <c r="K9" s="30">
+        <v>0</v>
+      </c>
+      <c r="L9" s="30">
+        <v>0</v>
+      </c>
       <c r="M9" s="30"/>
       <c r="N9" s="29"/>
       <c r="O9" s="29"/>
@@ -2428,7 +2436,7 @@
       <c r="AJ9" s="24"/>
       <c r="AK9" s="24"/>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.5">
       <c r="B10" s="18" t="s">
         <v>36</v>
       </c>
@@ -2454,8 +2462,12 @@
       <c r="J10" s="28">
         <v>0.95</v>
       </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
+      <c r="K10" s="30">
+        <v>0</v>
+      </c>
+      <c r="L10" s="30">
+        <v>0</v>
+      </c>
       <c r="M10" s="30"/>
       <c r="N10" s="29"/>
       <c r="O10" s="29"/>
@@ -2509,7 +2521,7 @@
       <c r="AJ10" s="24"/>
       <c r="AK10" s="24"/>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:37" x14ac:dyDescent="0.5">
       <c r="B11" s="18" t="s">
         <v>37</v>
       </c>
@@ -2535,8 +2547,12 @@
       <c r="J11" s="28">
         <v>0.95</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="K11" s="30">
+        <v>0</v>
+      </c>
+      <c r="L11" s="30">
+        <v>0</v>
+      </c>
       <c r="M11" s="30"/>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
@@ -2590,7 +2606,7 @@
       <c r="AJ11" s="24"/>
       <c r="AK11" s="24"/>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:37" x14ac:dyDescent="0.5">
       <c r="B12" s="18" t="s">
         <v>38</v>
       </c>
@@ -2616,8 +2632,12 @@
       <c r="J12" s="28">
         <v>0.95</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
+      <c r="K12" s="30">
+        <v>0</v>
+      </c>
+      <c r="L12" s="30">
+        <v>0</v>
+      </c>
       <c r="M12" s="30">
         <v>10</v>
       </c>
@@ -2673,7 +2693,7 @@
       <c r="AJ12" s="24"/>
       <c r="AK12" s="24"/>
     </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:37" x14ac:dyDescent="0.5">
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
@@ -2838,18 +2858,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2871,6 +2891,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2884,12 +2912,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement eStFinInterRes & eStFinIntraRes
</commit_message>
<xml_diff>
--- a/data/example/Power_Storage.xlsx
+++ b/data/example/Power_Storage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9955F5D4-CE8B-40BC-A702-014679118D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5E124E-0A23-4AB6-A859-727341C9754F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,15 +1429,21 @@
         <v>97</v>
       </c>
       <c r="F8" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14">
         <v>600</v>
       </c>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0.97</v>
+      </c>
+      <c r="K8" s="15">
+        <v>0.93</v>
+      </c>
       <c r="L8" s="15">
         <v>0</v>
       </c>
@@ -1456,11 +1462,21 @@
       <c r="Q8" s="13">
         <v>1</v>
       </c>
-      <c r="R8" s="15"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
+      <c r="R8" s="15">
+        <v>3</v>
+      </c>
+      <c r="S8" s="13">
+        <v>1</v>
+      </c>
+      <c r="T8" s="13">
+        <v>1</v>
+      </c>
+      <c r="U8" s="15">
+        <v>100</v>
+      </c>
+      <c r="V8" s="15">
+        <v>100</v>
+      </c>
       <c r="W8" s="14">
         <v>1600</v>
       </c>

</xml_diff>